<commit_message>
added ltc4359 ckt + components
</commit_message>
<xml_diff>
--- a/datasheets/components.xlsx
+++ b/datasheets/components.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tarko\Desktop\ece445\datasheets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bobox\Documents\_Documents\ece445\datasheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76DB7A6A-0E10-46EF-A5D6-7463AADCF8F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A54234AE-6249-4498-A88B-17C773BB04D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="56">
   <si>
     <t>Board</t>
   </si>
@@ -130,6 +130,69 @@
   </si>
   <si>
     <t>Don't know which package yet, maybe use optopisolation</t>
+  </si>
+  <si>
+    <t>Power Oring controller</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/analog-devices-inc/LTC4359CMS8-TRPBF/3306822</t>
+  </si>
+  <si>
+    <t>LTC4359CMS8#TRPBF</t>
+  </si>
+  <si>
+    <t>MOSFET</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/onsemi/NTBGS1D5N06C/14005228</t>
+  </si>
+  <si>
+    <t>NTBGS1D5N06C</t>
+  </si>
+  <si>
+    <t>Subsystem</t>
+  </si>
+  <si>
+    <t>3.3V buck</t>
+  </si>
+  <si>
+    <t>5V buck</t>
+  </si>
+  <si>
+    <t>Switching network</t>
+  </si>
+  <si>
+    <t>3.3V buck/5V buck</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/diodes-incorporated/SMAJ24CA-13-F/775748</t>
+  </si>
+  <si>
+    <t>TVS diode</t>
+  </si>
+  <si>
+    <t>SMAJ24CA-13-F</t>
+  </si>
+  <si>
+    <t>SMAJ58A</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/littelfuse-inc/SMAJ58A/762310</t>
+  </si>
+  <si>
+    <t>FDB13AN06A0</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/onsemi/FDB13AN06A0/978478</t>
+  </si>
+  <si>
+    <t>Zener diode</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/rohm-semiconductor/BZX84C12VLYT116/14682680</t>
+  </si>
+  <si>
+    <t>BZX84C12VLYT116</t>
   </si>
 </sst>
 </file>
@@ -480,244 +543,362 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F24"/>
+  <dimension ref="A1:G24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="22.6640625" customWidth="1"/>
-    <col min="3" max="3" width="30.6640625" customWidth="1"/>
-    <col min="4" max="4" width="101.5546875" customWidth="1"/>
-    <col min="5" max="5" width="11.5546875" customWidth="1"/>
-    <col min="6" max="6" width="36.44140625" customWidth="1"/>
+    <col min="2" max="2" width="20.28515625" customWidth="1"/>
+    <col min="3" max="3" width="27.28515625" customWidth="1"/>
+    <col min="4" max="4" width="30.7109375" customWidth="1"/>
+    <col min="5" max="5" width="112.42578125" customWidth="1"/>
+    <col min="6" max="6" width="11.5703125" customWidth="1"/>
+    <col min="7" max="7" width="36.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="G1" s="4" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="13.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
       <c r="B2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C2" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="D2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="E2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="5">
+      <c r="F2" s="5">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
       <c r="B3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C3" t="s">
         <v>3</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="E3" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="5"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F3" s="5"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
       <c r="B4" t="s">
+        <v>45</v>
+      </c>
+      <c r="C4" t="s">
         <v>14</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="E4" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="E4" s="5"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F4" s="5"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>2</v>
       </c>
       <c r="B5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C5" t="s">
         <v>19</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>18</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="E5" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="E5" s="5"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F5" s="5"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>2</v>
       </c>
       <c r="B6" t="s">
+        <v>45</v>
+      </c>
+      <c r="C6" t="s">
         <v>23</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>22</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="E6" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="E6" s="5"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F6" s="5"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>2</v>
       </c>
       <c r="B7" t="s">
+        <v>43</v>
+      </c>
+      <c r="C7" t="s">
         <v>16</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="D7" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="E7" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E7" s="5">
+      <c r="F7" s="5">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>2</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" t="s">
         <v>25</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D8" t="s">
         <v>27</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="E8" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="E8" s="6">
+      <c r="F8" s="6">
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>2</v>
       </c>
-      <c r="B9" t="s">
+      <c r="C9" t="s">
         <v>28</v>
       </c>
-      <c r="C9" t="s">
+      <c r="D9" t="s">
         <v>29</v>
       </c>
-      <c r="D9" s="3" t="s">
+      <c r="E9" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="E9" s="6">
+      <c r="F9" s="6">
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>2</v>
       </c>
-      <c r="B10" t="s">
+      <c r="C10" t="s">
         <v>31</v>
       </c>
-      <c r="C10" t="s">
+      <c r="D10" t="s">
         <v>32</v>
       </c>
-      <c r="D10" s="3" t="s">
+      <c r="E10" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="E10" s="6">
+      <c r="F10" s="6">
         <v>1</v>
       </c>
-      <c r="F10" t="s">
+      <c r="G10" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="E11" s="6"/>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="E12" s="6"/>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="E13" s="6"/>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="E14" s="6"/>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="E15" s="6"/>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="E16" s="6"/>
-    </row>
-    <row r="17" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E17" s="6"/>
-    </row>
-    <row r="18" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E18" s="6"/>
-    </row>
-    <row r="19" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E19" s="6"/>
-    </row>
-    <row r="20" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E20" s="6"/>
-    </row>
-    <row r="21" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E21" s="6"/>
-    </row>
-    <row r="22" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E22" s="6"/>
-    </row>
-    <row r="23" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E23" s="6"/>
-    </row>
-    <row r="24" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E24" s="6"/>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>2</v>
+      </c>
+      <c r="B11" t="s">
+        <v>44</v>
+      </c>
+      <c r="C11" t="s">
+        <v>35</v>
+      </c>
+      <c r="D11" t="s">
+        <v>37</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="F11" s="6"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>2</v>
+      </c>
+      <c r="B12" t="s">
+        <v>44</v>
+      </c>
+      <c r="C12" t="s">
+        <v>38</v>
+      </c>
+      <c r="D12" t="s">
+        <v>40</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="F12" s="6"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>2</v>
+      </c>
+      <c r="B13" t="s">
+        <v>44</v>
+      </c>
+      <c r="C13" t="s">
+        <v>47</v>
+      </c>
+      <c r="D13" t="s">
+        <v>48</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="F13" s="6"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>2</v>
+      </c>
+      <c r="B14" t="s">
+        <v>44</v>
+      </c>
+      <c r="C14" t="s">
+        <v>47</v>
+      </c>
+      <c r="D14" t="s">
+        <v>49</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="F14" s="6"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>2</v>
+      </c>
+      <c r="B15" t="s">
+        <v>44</v>
+      </c>
+      <c r="C15" t="s">
+        <v>38</v>
+      </c>
+      <c r="D15" t="s">
+        <v>51</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="F15" s="6"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>2</v>
+      </c>
+      <c r="B16" t="s">
+        <v>44</v>
+      </c>
+      <c r="C16" t="s">
+        <v>53</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="F16" s="6"/>
+    </row>
+    <row r="17" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F17" s="6"/>
+    </row>
+    <row r="18" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F18" s="6"/>
+    </row>
+    <row r="19" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F19" s="6"/>
+    </row>
+    <row r="20" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F20" s="6"/>
+    </row>
+    <row r="21" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F21" s="6"/>
+    </row>
+    <row r="22" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F22" s="6"/>
+    </row>
+    <row r="23" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F23" s="6"/>
+    </row>
+    <row r="24" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F24" s="6"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D6" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
-    <hyperlink ref="D5" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
-    <hyperlink ref="D4" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
-    <hyperlink ref="D7" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="D2" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="D3" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="D8" r:id="rId7" xr:uid="{1E41BAD6-12C0-46B0-B958-6378F93910CA}"/>
-    <hyperlink ref="D9" r:id="rId8" xr:uid="{0D350874-DACE-44D9-B49F-DAA00B5126BB}"/>
-    <hyperlink ref="D10" r:id="rId9" xr:uid="{5D176233-75E7-4A5C-8119-38F338C26FA8}"/>
+    <hyperlink ref="E6" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="E5" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="E4" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="E7" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="E2" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="E3" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="E8" r:id="rId7" xr:uid="{1E41BAD6-12C0-46B0-B958-6378F93910CA}"/>
+    <hyperlink ref="E9" r:id="rId8" xr:uid="{0D350874-DACE-44D9-B49F-DAA00B5126BB}"/>
+    <hyperlink ref="E10" r:id="rId9" xr:uid="{5D176233-75E7-4A5C-8119-38F338C26FA8}"/>
+    <hyperlink ref="E11" r:id="rId10" xr:uid="{9DA19847-C607-400E-A55E-69761C8165CF}"/>
+    <hyperlink ref="E12" r:id="rId11" xr:uid="{6DC79232-56CC-440D-BCDC-D5628F509F1A}"/>
+    <hyperlink ref="E13" r:id="rId12" xr:uid="{662DF471-323B-4E24-94B2-FEE367B7E46D}"/>
+    <hyperlink ref="E14" r:id="rId13" xr:uid="{2CE6164B-C192-4B1B-85D3-694E40FEEDD7}"/>
+    <hyperlink ref="E15" r:id="rId14" xr:uid="{6B22CEDA-37F2-4C5F-BAD8-0B24F05182E7}"/>
+    <hyperlink ref="E16" r:id="rId15" xr:uid="{A7CDDB75-A10B-4877-9AC9-82971EC83DD0}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId10"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId16"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added sensing components and mcu
</commit_message>
<xml_diff>
--- a/datasheets/components.xlsx
+++ b/datasheets/components.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tarko\Desktop\ece445\datasheets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ry5iu\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{807A081E-35D6-406C-A984-CBF8B4EA118A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0035894E-3493-4C84-A188-12701C847631}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3075" yWindow="3075" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="94">
   <si>
     <t>Board</t>
   </si>
@@ -268,13 +268,52 @@
   </si>
   <si>
     <t>Maybe? Might design one instead</t>
+  </si>
+  <si>
+    <t>Sensing</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/adafruit-industries-llc/161/7244927?utm_adgroup=Optical%20Sensors%20-%20Photo%20Detectors%20-%20CdS%20Cells&amp;utm_source=google&amp;utm_medium=cpc&amp;utm_campaign=Shopping_Product_Sensors%2C%20Transducers&amp;utm_term=&amp;utm_content=Optical%20Sensors%20-%20Photo%20Detectors%20-%20CdS%20Cells&amp;gclid=Cj0KCQiA09eQBhCxARIsAAYRiykKKTy26t9RMu3thm4BXJjP05883nAXP3698XRbwioa7IpavDa5CJsaAmxBEALw_wcB</t>
+  </si>
+  <si>
+    <t>photoresistor</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/microchip-technology/ATMEGA328-PU/2271026</t>
+  </si>
+  <si>
+    <t>MCU</t>
+  </si>
+  <si>
+    <t>ATMEGA328-PU</t>
+  </si>
+  <si>
+    <t>Humidity sensor</t>
+  </si>
+  <si>
+    <t>DHT20</t>
+  </si>
+  <si>
+    <t>https://www.sparkfun.com/products/18364</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/sharp-socle-technology/GP2Y0A710K0F/2117639</t>
+  </si>
+  <si>
+    <t>IR sensor</t>
+  </si>
+  <si>
+    <t>GP2Y0A710K0F</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -295,6 +334,11 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF222222"/>
+      <name val="Roboto"/>
     </font>
   </fonts>
   <fills count="2">
@@ -327,7 +371,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -337,6 +381,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -618,23 +666,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G24"/>
+  <dimension ref="A1:G27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G25" sqref="G25"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="20.33203125" customWidth="1"/>
-    <col min="3" max="3" width="27.33203125" customWidth="1"/>
-    <col min="4" max="4" width="30.6640625" customWidth="1"/>
-    <col min="5" max="5" width="112.44140625" customWidth="1"/>
-    <col min="6" max="6" width="11.5546875" customWidth="1"/>
-    <col min="7" max="7" width="36.44140625" customWidth="1"/>
+    <col min="2" max="2" width="20.28515625" customWidth="1"/>
+    <col min="3" max="3" width="27.28515625" customWidth="1"/>
+    <col min="4" max="4" width="30.7109375" customWidth="1"/>
+    <col min="5" max="5" width="112.42578125" customWidth="1"/>
+    <col min="6" max="6" width="11.5703125" customWidth="1"/>
+    <col min="7" max="7" width="36.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -657,7 +705,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="13.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -677,7 +725,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -695,7 +743,7 @@
       </c>
       <c r="F3" s="5"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -713,7 +761,7 @@
       </c>
       <c r="F4" s="5"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -731,7 +779,7 @@
       </c>
       <c r="F5" s="5"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>2</v>
       </c>
@@ -749,7 +797,7 @@
       </c>
       <c r="F6" s="5"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>2</v>
       </c>
@@ -769,7 +817,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>2</v>
       </c>
@@ -792,7 +840,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>2</v>
       </c>
@@ -812,7 +860,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>2</v>
       </c>
@@ -835,7 +883,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>2</v>
       </c>
@@ -853,7 +901,7 @@
       </c>
       <c r="F11" s="6"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>2</v>
       </c>
@@ -871,7 +919,7 @@
       </c>
       <c r="F12" s="6"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>2</v>
       </c>
@@ -889,7 +937,7 @@
       </c>
       <c r="F13" s="6"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>2</v>
       </c>
@@ -907,7 +955,7 @@
       </c>
       <c r="F14" s="6"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>2</v>
       </c>
@@ -925,7 +973,7 @@
       </c>
       <c r="F15" s="6"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>2</v>
       </c>
@@ -945,7 +993,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>52</v>
       </c>
@@ -965,7 +1013,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>52</v>
       </c>
@@ -985,7 +1033,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>52</v>
       </c>
@@ -1008,7 +1056,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>52</v>
       </c>
@@ -1031,7 +1079,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>52</v>
       </c>
@@ -1054,7 +1102,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>52</v>
       </c>
@@ -1077,7 +1125,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>2</v>
       </c>
@@ -1100,8 +1148,74 @@
         <v>80</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>82</v>
+      </c>
+      <c r="B24" t="s">
+        <v>81</v>
+      </c>
+      <c r="C24" t="s">
+        <v>84</v>
+      </c>
+      <c r="D24" s="8">
+        <v>161</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>83</v>
+      </c>
       <c r="F24" s="6"/>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>82</v>
+      </c>
+      <c r="B25" t="s">
+        <v>81</v>
+      </c>
+      <c r="C25" t="s">
+        <v>88</v>
+      </c>
+      <c r="D25" t="s">
+        <v>89</v>
+      </c>
+      <c r="E25" s="3" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>82</v>
+      </c>
+      <c r="B26" t="s">
+        <v>81</v>
+      </c>
+      <c r="C26" t="s">
+        <v>92</v>
+      </c>
+      <c r="D26" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="E26" s="3" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>82</v>
+      </c>
+      <c r="B27" t="s">
+        <v>86</v>
+      </c>
+      <c r="C27" t="s">
+        <v>86</v>
+      </c>
+      <c r="D27" t="s">
+        <v>87</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>85</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
@@ -1127,8 +1241,12 @@
     <hyperlink ref="E21" r:id="rId20" xr:uid="{4CABAE57-840F-4A28-A31A-B225DD610105}"/>
     <hyperlink ref="E22" r:id="rId21" xr:uid="{D305F5B0-2959-4350-95CD-DAD660A2D24E}"/>
     <hyperlink ref="E23" r:id="rId22" xr:uid="{F3522BF4-7A73-41BF-B0F6-8FB642D1752C}"/>
+    <hyperlink ref="E24" r:id="rId23" display="https://www.digikey.com/en/products/detail/adafruit-industries-llc/161/7244927?utm_adgroup=Optical%20Sensors%20-%20Photo%20Detectors%20-%20CdS%20Cells&amp;utm_source=google&amp;utm_medium=cpc&amp;utm_campaign=Shopping_Product_Sensors%2C%20Transducers&amp;utm_term=&amp;utm_content=Optical%20Sensors%20-%20Photo%20Detectors%20-%20CdS%20Cells&amp;gclid=Cj0KCQiA09eQBhCxARIsAAYRiykKKTy26t9RMu3thm4BXJjP05883nAXP3698XRbwioa7IpavDa5CJsaAmxBEALw_wcB" xr:uid="{6190C92F-9862-4533-AD39-13A7CC373B2E}"/>
+    <hyperlink ref="E27" r:id="rId24" xr:uid="{FACFA13F-07A7-47F1-8A04-C0060C0169F5}"/>
+    <hyperlink ref="E25" r:id="rId25" xr:uid="{6331C730-E1DC-4649-B910-B37561FE0D25}"/>
+    <hyperlink ref="E26" r:id="rId26" xr:uid="{178B6D46-AD3D-413F-8053-934E284D654E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId23"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId27"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
screenshots and adding components
</commit_message>
<xml_diff>
--- a/datasheets/components.xlsx
+++ b/datasheets/components.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tarko\Desktop\ece445\datasheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{080786F4-1D43-47F2-B93C-44B2CFE5B402}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F617FEE-2D83-481A-A293-498173E1446A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9900" yWindow="2340" windowWidth="16728" windowHeight="10908" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="101">
   <si>
     <t>Board</t>
   </si>
@@ -105,18 +105,9 @@
     <t>Power Monitor (I2C)</t>
   </si>
   <si>
-    <t>Power Oring controller</t>
-  </si>
-  <si>
     <t>MOSFET</t>
   </si>
   <si>
-    <t>https://www.digikey.com/en/products/detail/onsemi/NTBGS1D5N06C/14005228</t>
-  </si>
-  <si>
-    <t>NTBGS1D5N06C</t>
-  </si>
-  <si>
     <t>Subsystem</t>
   </si>
   <si>
@@ -126,54 +117,15 @@
     <t>5V buck</t>
   </si>
   <si>
-    <t>Switching network</t>
-  </si>
-  <si>
     <t>3.3V buck/5V buck</t>
   </si>
   <si>
-    <t>https://www.digikey.com/en/products/detail/diodes-incorporated/SMAJ24CA-13-F/775748</t>
-  </si>
-  <si>
-    <t>TVS diode</t>
-  </si>
-  <si>
-    <t>SMAJ24CA-13-F</t>
-  </si>
-  <si>
-    <t>SMAJ58A</t>
-  </si>
-  <si>
-    <t>https://www.digikey.com/en/products/detail/littelfuse-inc/SMAJ58A/762310</t>
-  </si>
-  <si>
-    <t>FDB13AN06A0</t>
-  </si>
-  <si>
-    <t>https://www.digikey.com/en/products/detail/onsemi/FDB13AN06A0/978478</t>
-  </si>
-  <si>
-    <t>Zener diode</t>
-  </si>
-  <si>
-    <t>https://www.digikey.com/en/products/detail/rohm-semiconductor/BZX84C12VLYT116/14682680</t>
-  </si>
-  <si>
-    <t>BZX84C12VLYT116</t>
-  </si>
-  <si>
     <t>Solar</t>
   </si>
   <si>
     <t>120VAC/24VDC</t>
   </si>
   <si>
-    <t>LTC4359IS8#PBF</t>
-  </si>
-  <si>
-    <t>https://www.digikey.com/en/products/detail/analog-devices-inc/LTC4359IS8-PBF/9586593</t>
-  </si>
-  <si>
     <t>LTC4151IMS-1#TRPBF</t>
   </si>
   <si>
@@ -204,9 +156,6 @@
     <t>https://www.digikey.com/en/products/detail/panasonic-electronic-components/ERJ-3BWFR020V/5647494</t>
   </si>
   <si>
-    <t>Already have (plus spare)</t>
-  </si>
-  <si>
     <t>Needs heat sink</t>
   </si>
   <si>
@@ -355,6 +304,30 @@
   </si>
   <si>
     <t>22uF Electrolytic Capacitor</t>
+  </si>
+  <si>
+    <t>DC/DC Controller</t>
+  </si>
+  <si>
+    <t>LT3757AIMSE#PBF</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/analog-devices-inc/LT3757AIMSE-PBF/3838483</t>
+  </si>
+  <si>
+    <t>Switching Network</t>
+  </si>
+  <si>
+    <t>1 uF capacitor</t>
+  </si>
+  <si>
+    <t>FDD8453LZ</t>
+  </si>
+  <si>
+    <t>Quad High-Side Gate Driver</t>
+  </si>
+  <si>
+    <t>LT1161IN#PBF</t>
   </si>
 </sst>
 </file>
@@ -714,10 +687,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G36"/>
+  <dimension ref="A1:G42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C18" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -735,7 +708,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
@@ -758,7 +731,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C2" t="s">
         <v>15</v>
@@ -778,7 +751,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C3" t="s">
         <v>3</v>
@@ -796,7 +769,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C4" t="s">
         <v>14</v>
@@ -814,7 +787,7 @@
         <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C5" t="s">
         <v>19</v>
@@ -832,7 +805,7 @@
         <v>2</v>
       </c>
       <c r="B6" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C6" t="s">
         <v>23</v>
@@ -850,7 +823,7 @@
         <v>2</v>
       </c>
       <c r="B7" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C7" t="s">
         <v>16</v>
@@ -870,22 +843,22 @@
         <v>2</v>
       </c>
       <c r="B8" t="s">
+        <v>31</v>
+      </c>
+      <c r="C8" t="s">
+        <v>44</v>
+      </c>
+      <c r="D8" t="s">
         <v>45</v>
       </c>
-      <c r="C8" t="s">
-        <v>61</v>
-      </c>
-      <c r="D8" t="s">
-        <v>62</v>
-      </c>
       <c r="E8" s="3" t="s">
-        <v>63</v>
+        <v>46</v>
       </c>
       <c r="F8" s="6">
         <v>1</v>
       </c>
       <c r="G8" t="s">
-        <v>60</v>
+        <v>43</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
@@ -893,16 +866,16 @@
         <v>2</v>
       </c>
       <c r="B9" t="s">
-        <v>46</v>
+        <v>32</v>
       </c>
       <c r="C9" t="s">
-        <v>64</v>
+        <v>47</v>
       </c>
       <c r="D9" t="s">
-        <v>66</v>
+        <v>49</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>65</v>
+        <v>48</v>
       </c>
       <c r="F9" s="6">
         <v>1</v>
@@ -913,195 +886,196 @@
         <v>2</v>
       </c>
       <c r="B10" t="s">
+        <v>35</v>
+      </c>
+      <c r="C10" t="s">
+        <v>25</v>
+      </c>
+      <c r="D10" t="s">
         <v>33</v>
       </c>
-      <c r="C10" t="s">
-        <v>26</v>
-      </c>
-      <c r="D10" t="s">
-        <v>47</v>
-      </c>
       <c r="E10" s="3" t="s">
-        <v>48</v>
+        <v>34</v>
       </c>
       <c r="F10" s="6">
-        <v>2</v>
-      </c>
-      <c r="G10" t="s">
-        <v>59</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>2</v>
+        <v>36</v>
       </c>
       <c r="B11" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C11" t="s">
-        <v>27</v>
+        <v>37</v>
       </c>
       <c r="D11" t="s">
-        <v>29</v>
+        <v>38</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="F11" s="6"/>
+        <v>39</v>
+      </c>
+      <c r="F11" s="6">
+        <v>2</v>
+      </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>2</v>
+        <v>36</v>
       </c>
       <c r="B12" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C12" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="D12" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="F12" s="6"/>
+        <v>42</v>
+      </c>
+      <c r="F12" s="6">
+        <v>1</v>
+      </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>2</v>
+        <v>51</v>
       </c>
       <c r="B13" t="s">
-        <v>33</v>
+        <v>50</v>
       </c>
       <c r="C13" t="s">
-        <v>36</v>
-      </c>
-      <c r="D13" t="s">
-        <v>38</v>
+        <v>53</v>
+      </c>
+      <c r="D13" s="8">
+        <v>161</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>39</v>
+        <v>52</v>
       </c>
       <c r="F13" s="6"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>2</v>
+        <v>51</v>
       </c>
       <c r="B14" t="s">
-        <v>33</v>
+        <v>50</v>
       </c>
       <c r="C14" t="s">
-        <v>27</v>
+        <v>57</v>
       </c>
       <c r="D14" t="s">
-        <v>40</v>
+        <v>58</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="F14" s="6"/>
+        <v>59</v>
+      </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>2</v>
+        <v>51</v>
       </c>
       <c r="B15" t="s">
-        <v>33</v>
+        <v>50</v>
       </c>
       <c r="C15" t="s">
-        <v>42</v>
-      </c>
-      <c r="D15" s="5" t="s">
-        <v>44</v>
+        <v>61</v>
+      </c>
+      <c r="D15" s="7" t="s">
+        <v>62</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="F15" s="6"/>
+        <v>60</v>
+      </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>2</v>
+        <v>51</v>
       </c>
       <c r="B16" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C16" t="s">
-        <v>25</v>
+        <v>64</v>
       </c>
       <c r="D16" t="s">
-        <v>49</v>
+        <v>65</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="F16" s="6">
-        <v>1</v>
+        <v>63</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B17" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="C17" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="D17" t="s">
+        <v>56</v>
+      </c>
+      <c r="E17" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="E17" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="F17" s="6">
-        <v>2</v>
+      <c r="F17">
+        <v>1</v>
+      </c>
+      <c r="G17" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>52</v>
+        <v>2</v>
       </c>
       <c r="B18" t="s">
-        <v>51</v>
+        <v>67</v>
       </c>
       <c r="C18" t="s">
-        <v>56</v>
+        <v>68</v>
       </c>
       <c r="D18" t="s">
-        <v>57</v>
+        <v>69</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="F18" s="6">
+        <v>70</v>
+      </c>
+      <c r="F18">
         <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>68</v>
+        <v>2</v>
       </c>
       <c r="B19" t="s">
         <v>67</v>
       </c>
       <c r="C19" t="s">
-        <v>70</v>
-      </c>
-      <c r="D19" s="8">
-        <v>161</v>
+        <v>71</v>
+      </c>
+      <c r="D19" t="s">
+        <v>73</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="F19" s="6"/>
+        <v>72</v>
+      </c>
+      <c r="F19">
+        <v>1</v>
+      </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>68</v>
+        <v>2</v>
       </c>
       <c r="B20" t="s">
         <v>67</v>
@@ -1115,62 +1089,68 @@
       <c r="E20" s="3" t="s">
         <v>76</v>
       </c>
+      <c r="F20">
+        <v>1</v>
+      </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>68</v>
+        <v>2</v>
       </c>
       <c r="B21" t="s">
         <v>67</v>
       </c>
       <c r="C21" t="s">
+        <v>26</v>
+      </c>
+      <c r="D21" t="s">
+        <v>77</v>
+      </c>
+      <c r="E21" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="D21" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="E21" s="3" t="s">
-        <v>77</v>
+      <c r="F21">
+        <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>68</v>
+        <v>2</v>
       </c>
       <c r="B22" t="s">
         <v>67</v>
       </c>
       <c r="C22" t="s">
+        <v>79</v>
+      </c>
+      <c r="D22" t="s">
+        <v>80</v>
+      </c>
+      <c r="E22" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="D22" t="s">
-        <v>82</v>
-      </c>
-      <c r="E22" s="3" t="s">
-        <v>80</v>
+      <c r="F22">
+        <v>4</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>68</v>
+        <v>2</v>
       </c>
       <c r="B23" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="C23" t="s">
-        <v>72</v>
+        <v>82</v>
       </c>
       <c r="D23" t="s">
-        <v>73</v>
+        <v>83</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>71</v>
+        <v>84</v>
       </c>
       <c r="F23">
         <v>1</v>
-      </c>
-      <c r="G23" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
@@ -1178,7 +1158,7 @@
         <v>2</v>
       </c>
       <c r="B24" t="s">
-        <v>84</v>
+        <v>67</v>
       </c>
       <c r="C24" t="s">
         <v>85</v>
@@ -1198,13 +1178,13 @@
         <v>2</v>
       </c>
       <c r="B25" t="s">
-        <v>84</v>
+        <v>67</v>
       </c>
       <c r="C25" t="s">
+        <v>3</v>
+      </c>
+      <c r="D25" t="s">
         <v>88</v>
-      </c>
-      <c r="D25" t="s">
-        <v>90</v>
       </c>
       <c r="E25" s="3" t="s">
         <v>89</v>
@@ -1218,19 +1198,19 @@
         <v>2</v>
       </c>
       <c r="B26" t="s">
-        <v>84</v>
+        <v>67</v>
       </c>
       <c r="C26" t="s">
+        <v>92</v>
+      </c>
+      <c r="D26" t="s">
+        <v>90</v>
+      </c>
+      <c r="E26" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="D26" t="s">
-        <v>92</v>
-      </c>
-      <c r="E26" s="3" t="s">
-        <v>93</v>
-      </c>
       <c r="F26">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.3">
@@ -1238,10 +1218,10 @@
         <v>2</v>
       </c>
       <c r="B27" t="s">
-        <v>84</v>
+        <v>67</v>
       </c>
       <c r="C27" t="s">
-        <v>27</v>
+        <v>93</v>
       </c>
       <c r="D27" t="s">
         <v>94</v>
@@ -1258,19 +1238,13 @@
         <v>2</v>
       </c>
       <c r="B28" t="s">
-        <v>84</v>
+        <v>96</v>
       </c>
       <c r="C28" t="s">
-        <v>96</v>
-      </c>
-      <c r="D28" t="s">
         <v>97</v>
       </c>
-      <c r="E28" s="3" t="s">
-        <v>98</v>
-      </c>
       <c r="F28">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.3">
@@ -1278,19 +1252,16 @@
         <v>2</v>
       </c>
       <c r="B29" t="s">
-        <v>84</v>
+        <v>96</v>
       </c>
       <c r="C29" t="s">
-        <v>99</v>
+        <v>26</v>
       </c>
       <c r="D29" t="s">
-        <v>100</v>
-      </c>
-      <c r="E29" s="3" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="F29">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.3">
@@ -1298,91 +1269,76 @@
         <v>2</v>
       </c>
       <c r="B30" t="s">
-        <v>84</v>
+        <v>96</v>
       </c>
       <c r="C30" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="D30" t="s">
-        <v>103</v>
-      </c>
-      <c r="E30" s="3" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="F30">
         <v>1</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A31" t="s">
-        <v>2</v>
-      </c>
       <c r="B31" t="s">
-        <v>84</v>
-      </c>
-      <c r="C31" t="s">
-        <v>3</v>
-      </c>
-      <c r="D31" t="s">
-        <v>105</v>
-      </c>
-      <c r="E31" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="F31">
-        <v>1</v>
+        <v>96</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A32" t="s">
-        <v>2</v>
-      </c>
       <c r="B32" t="s">
-        <v>84</v>
-      </c>
-      <c r="C32" t="s">
-        <v>109</v>
-      </c>
-      <c r="D32" t="s">
-        <v>107</v>
-      </c>
-      <c r="E32" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="F32">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A33" t="s">
-        <v>2</v>
-      </c>
+        <v>96</v>
+      </c>
+    </row>
+    <row r="33" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B33" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A34" t="s">
-        <v>2</v>
-      </c>
+        <v>96</v>
+      </c>
+    </row>
+    <row r="34" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B34" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A35" t="s">
-        <v>2</v>
-      </c>
+        <v>96</v>
+      </c>
+    </row>
+    <row r="35" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B35" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A36" t="s">
-        <v>2</v>
-      </c>
+        <v>96</v>
+      </c>
+    </row>
+    <row r="36" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B36" t="s">
-        <v>84</v>
+        <v>96</v>
+      </c>
+    </row>
+    <row r="37" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B37" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="38" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B38" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="39" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B39" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="40" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B40" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="41" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B41" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="42" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B42" t="s">
+        <v>96</v>
       </c>
     </row>
   </sheetData>
@@ -1395,31 +1351,26 @@
     <hyperlink ref="E3" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
     <hyperlink ref="E8" r:id="rId7" xr:uid="{1E41BAD6-12C0-46B0-B958-6378F93910CA}"/>
     <hyperlink ref="E9" r:id="rId8" xr:uid="{0D350874-DACE-44D9-B49F-DAA00B5126BB}"/>
-    <hyperlink ref="E10" r:id="rId9" xr:uid="{9DA19847-C607-400E-A55E-69761C8165CF}"/>
-    <hyperlink ref="E11" r:id="rId10" xr:uid="{6DC79232-56CC-440D-BCDC-D5628F509F1A}"/>
-    <hyperlink ref="E12" r:id="rId11" xr:uid="{662DF471-323B-4E24-94B2-FEE367B7E46D}"/>
-    <hyperlink ref="E13" r:id="rId12" xr:uid="{2CE6164B-C192-4B1B-85D3-694E40FEEDD7}"/>
-    <hyperlink ref="E14" r:id="rId13" xr:uid="{6B22CEDA-37F2-4C5F-BAD8-0B24F05182E7}"/>
-    <hyperlink ref="E15" r:id="rId14" xr:uid="{A7CDDB75-A10B-4877-9AC9-82971EC83DD0}"/>
-    <hyperlink ref="E16" r:id="rId15" xr:uid="{22DAAB31-6CD7-4550-8D7B-BA5AC511D404}"/>
-    <hyperlink ref="E17" r:id="rId16" xr:uid="{701FE240-7248-4EDC-98EB-224AFC9E35B7}"/>
-    <hyperlink ref="E18" r:id="rId17" xr:uid="{33A26128-8B39-4D5D-9794-2EE679C5480F}"/>
-    <hyperlink ref="E19" r:id="rId18" display="https://www.digikey.com/en/products/detail/adafruit-industries-llc/161/7244927?utm_adgroup=Optical%20Sensors%20-%20Photo%20Detectors%20-%20CdS%20Cells&amp;utm_source=google&amp;utm_medium=cpc&amp;utm_campaign=Shopping_Product_Sensors%2C%20Transducers&amp;utm_term=&amp;utm_content=Optical%20Sensors%20-%20Photo%20Detectors%20-%20CdS%20Cells&amp;gclid=Cj0KCQiA09eQBhCxARIsAAYRiykKKTy26t9RMu3thm4BXJjP05883nAXP3698XRbwioa7IpavDa5CJsaAmxBEALw_wcB" xr:uid="{6190C92F-9862-4533-AD39-13A7CC373B2E}"/>
-    <hyperlink ref="E23" r:id="rId19" xr:uid="{FACFA13F-07A7-47F1-8A04-C0060C0169F5}"/>
-    <hyperlink ref="E20" r:id="rId20" xr:uid="{6331C730-E1DC-4649-B910-B37561FE0D25}"/>
-    <hyperlink ref="E21" r:id="rId21" xr:uid="{178B6D46-AD3D-413F-8053-934E284D654E}"/>
-    <hyperlink ref="E22" r:id="rId22" xr:uid="{C4D3C7CE-F535-43A1-AB91-37A97CE9D29F}"/>
-    <hyperlink ref="E24" r:id="rId23" xr:uid="{A0FACEA3-0B20-4127-831C-02FEC6E8E50F}"/>
-    <hyperlink ref="E25" r:id="rId24" xr:uid="{E27363C6-A88C-4270-9B3D-D95CBCAFDE59}"/>
-    <hyperlink ref="E26" r:id="rId25" xr:uid="{02CB4450-EBEC-4C26-BB05-20C384B3FEB5}"/>
-    <hyperlink ref="E27" r:id="rId26" xr:uid="{F7F54A49-3154-4E9D-AD1E-D98B10CEE5A3}"/>
-    <hyperlink ref="E28" r:id="rId27" xr:uid="{3C4A0AD3-D018-4F45-8DCB-EC3A8C641D01}"/>
-    <hyperlink ref="E29" r:id="rId28" xr:uid="{E4DE17AA-C66E-4E64-A6B1-EFB138B489D0}"/>
-    <hyperlink ref="E30" r:id="rId29" xr:uid="{E37D2F7F-7E62-4320-9C57-2DE6916AB50A}"/>
-    <hyperlink ref="E31" r:id="rId30" xr:uid="{30D9FFE1-0745-430C-BACD-3FA6B8B712E4}"/>
-    <hyperlink ref="E32" r:id="rId31" xr:uid="{71CFCE49-06E9-4816-9DD2-CBF9DAE9561B}"/>
+    <hyperlink ref="E10" r:id="rId9" xr:uid="{22DAAB31-6CD7-4550-8D7B-BA5AC511D404}"/>
+    <hyperlink ref="E11" r:id="rId10" xr:uid="{701FE240-7248-4EDC-98EB-224AFC9E35B7}"/>
+    <hyperlink ref="E12" r:id="rId11" xr:uid="{33A26128-8B39-4D5D-9794-2EE679C5480F}"/>
+    <hyperlink ref="E13" r:id="rId12" display="https://www.digikey.com/en/products/detail/adafruit-industries-llc/161/7244927?utm_adgroup=Optical%20Sensors%20-%20Photo%20Detectors%20-%20CdS%20Cells&amp;utm_source=google&amp;utm_medium=cpc&amp;utm_campaign=Shopping_Product_Sensors%2C%20Transducers&amp;utm_term=&amp;utm_content=Optical%20Sensors%20-%20Photo%20Detectors%20-%20CdS%20Cells&amp;gclid=Cj0KCQiA09eQBhCxARIsAAYRiykKKTy26t9RMu3thm4BXJjP05883nAXP3698XRbwioa7IpavDa5CJsaAmxBEALw_wcB" xr:uid="{6190C92F-9862-4533-AD39-13A7CC373B2E}"/>
+    <hyperlink ref="E17" r:id="rId13" xr:uid="{FACFA13F-07A7-47F1-8A04-C0060C0169F5}"/>
+    <hyperlink ref="E14" r:id="rId14" xr:uid="{6331C730-E1DC-4649-B910-B37561FE0D25}"/>
+    <hyperlink ref="E15" r:id="rId15" xr:uid="{178B6D46-AD3D-413F-8053-934E284D654E}"/>
+    <hyperlink ref="E16" r:id="rId16" xr:uid="{C4D3C7CE-F535-43A1-AB91-37A97CE9D29F}"/>
+    <hyperlink ref="E18" r:id="rId17" xr:uid="{A0FACEA3-0B20-4127-831C-02FEC6E8E50F}"/>
+    <hyperlink ref="E19" r:id="rId18" xr:uid="{E27363C6-A88C-4270-9B3D-D95CBCAFDE59}"/>
+    <hyperlink ref="E20" r:id="rId19" xr:uid="{02CB4450-EBEC-4C26-BB05-20C384B3FEB5}"/>
+    <hyperlink ref="E21" r:id="rId20" xr:uid="{F7F54A49-3154-4E9D-AD1E-D98B10CEE5A3}"/>
+    <hyperlink ref="E22" r:id="rId21" xr:uid="{3C4A0AD3-D018-4F45-8DCB-EC3A8C641D01}"/>
+    <hyperlink ref="E23" r:id="rId22" xr:uid="{E4DE17AA-C66E-4E64-A6B1-EFB138B489D0}"/>
+    <hyperlink ref="E24" r:id="rId23" xr:uid="{E37D2F7F-7E62-4320-9C57-2DE6916AB50A}"/>
+    <hyperlink ref="E25" r:id="rId24" xr:uid="{30D9FFE1-0745-430C-BACD-3FA6B8B712E4}"/>
+    <hyperlink ref="E26" r:id="rId25" xr:uid="{71CFCE49-06E9-4816-9DD2-CBF9DAE9561B}"/>
+    <hyperlink ref="E27" r:id="rId26" xr:uid="{69F6B220-300E-4313-875C-BDA2A9162BA2}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId32"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId27"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added isolation to power and light boards
</commit_message>
<xml_diff>
--- a/datasheets/components.xlsx
+++ b/datasheets/components.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="9900" yWindow="2340" windowWidth="16725" windowHeight="10905" activeTab="1"/>
+    <workbookView xWindow="9900" yWindow="2340" windowWidth="16725" windowHeight="10905"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="332" uniqueCount="177">
   <si>
     <t>Board</t>
   </si>
@@ -120,12 +120,6 @@
     <t>3.3V buck/5V buck</t>
   </si>
   <si>
-    <t>Solar</t>
-  </si>
-  <si>
-    <t>120VAC/24VDC</t>
-  </si>
-  <si>
     <t>LTC4151IMS-1#TRPBF</t>
   </si>
   <si>
@@ -138,15 +132,9 @@
     <t xml:space="preserve">Power </t>
   </si>
   <si>
-    <t>Optoisolator</t>
-  </si>
-  <si>
     <t>MOCD207M</t>
   </si>
   <si>
-    <t>https://www.digikey.com/en/products/detail/onsemi/MOCD207M/281247</t>
-  </si>
-  <si>
     <t>Sense Resistor</t>
   </si>
   <si>
@@ -156,21 +144,12 @@
     <t>https://www.digikey.com/en/products/detail/panasonic-electronic-components/ERJ-3BWFR020V/5647494</t>
   </si>
   <si>
-    <t>Needs heat sink</t>
-  </si>
-  <si>
-    <t>140W (33 Ohm) Resistor</t>
-  </si>
-  <si>
     <t>TEH140M33R0FE</t>
   </si>
   <si>
     <t>https://www.mouser.com/ProductDetail/Ohmite/TEH140M33R0FE?qs=r5DSvlrkXmJ6291snezuUw%3D%3D</t>
   </si>
   <si>
-    <t>100W AC/DC Converter</t>
-  </si>
-  <si>
     <t>https://www.digikey.com/en/products/detail/mornsun-america-llc/LM100-23B24/13168375</t>
   </si>
   <si>
@@ -514,6 +493,69 @@
   </si>
   <si>
     <t>https://www.digikey.com/en/products/detail/te-connectivity-potter-brumfield-relays/1462041-7/2126941</t>
+  </si>
+  <si>
+    <t>optoisolator</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/fairchild-semiconductor/MOCD207M/281247</t>
+  </si>
+  <si>
+    <t>RMCF0603JT5K10</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/stackpole-electronics-inc/RMCF0603JT5K10/1757959</t>
+  </si>
+  <si>
+    <t>5.1k res</t>
+  </si>
+  <si>
+    <t>510 res</t>
+  </si>
+  <si>
+    <t>ESR10EZPJ511</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/rohm-semiconductor/ESR10EZPJ511/1762828</t>
+  </si>
+  <si>
+    <t>RMCF0805JT10K0</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/stackpole-electronics-inc/RMCF0805JT10K0/1757762</t>
+  </si>
+  <si>
+    <t>Buttons</t>
+  </si>
+  <si>
+    <t>33 power res</t>
+  </si>
+  <si>
+    <t>100k res</t>
+  </si>
+  <si>
+    <t>RMCF1206JT100K</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/stackpole-electronics-inc/RMCF1206JT100K/1757423</t>
+  </si>
+  <si>
+    <t>button</t>
+  </si>
+  <si>
+    <t>GPTS203211B</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/cw-industries/GPTS203211B/3190590</t>
+  </si>
+  <si>
+    <t>power res heat sink</t>
+  </si>
+  <si>
+    <t>588-E2A-T247-38E</t>
+  </si>
+  <si>
+    <t>https://www.mouser.com/ProductDetail/588-E2A-T247-38E</t>
   </si>
 </sst>
 </file>
@@ -948,8 +990,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G27"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10:F12"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8:G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1012,198 +1054,115 @@
       <c r="F7" s="5"/>
     </row>
     <row r="8" spans="1:7">
-      <c r="A8" t="s">
-        <v>2</v>
-      </c>
-      <c r="B8" t="s">
-        <v>31</v>
-      </c>
-      <c r="C8" t="s">
-        <v>44</v>
-      </c>
-      <c r="D8" t="s">
-        <v>45</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="F8" s="6">
-        <v>1</v>
-      </c>
-      <c r="G8" t="s">
-        <v>43</v>
-      </c>
+      <c r="E8" s="3"/>
+      <c r="F8" s="6"/>
     </row>
     <row r="9" spans="1:7">
-      <c r="A9" t="s">
-        <v>2</v>
-      </c>
-      <c r="B9" t="s">
-        <v>32</v>
-      </c>
-      <c r="C9" t="s">
-        <v>47</v>
-      </c>
-      <c r="D9" t="s">
-        <v>49</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="F9" s="6">
-        <v>1</v>
-      </c>
+      <c r="E9" s="3"/>
+      <c r="F9" s="6"/>
     </row>
     <row r="10" spans="1:7">
-      <c r="A10" t="s">
-        <v>2</v>
-      </c>
-      <c r="B10" t="s">
-        <v>35</v>
-      </c>
-      <c r="C10" t="s">
-        <v>25</v>
-      </c>
-      <c r="D10" t="s">
-        <v>33</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="F10" s="6">
-        <v>1</v>
-      </c>
+      <c r="E10" s="3"/>
+      <c r="F10" s="6"/>
     </row>
     <row r="11" spans="1:7">
-      <c r="A11" t="s">
-        <v>36</v>
-      </c>
-      <c r="B11" t="s">
-        <v>35</v>
-      </c>
-      <c r="C11" t="s">
-        <v>37</v>
-      </c>
-      <c r="D11" t="s">
-        <v>38</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="F11" s="6">
-        <v>2</v>
-      </c>
+      <c r="E11" s="3"/>
+      <c r="F11" s="6"/>
     </row>
     <row r="12" spans="1:7">
-      <c r="A12" t="s">
-        <v>36</v>
-      </c>
-      <c r="B12" t="s">
-        <v>35</v>
-      </c>
-      <c r="C12" t="s">
-        <v>40</v>
-      </c>
-      <c r="D12" t="s">
-        <v>41</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="F12" s="6">
-        <v>1</v>
-      </c>
+      <c r="E12" s="3"/>
+      <c r="F12" s="6"/>
     </row>
     <row r="13" spans="1:7">
       <c r="A13" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="B13" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="C13" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="D13" s="8">
         <v>161</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="F13" s="6"/>
     </row>
     <row r="14" spans="1:7">
       <c r="A14" t="s">
+        <v>44</v>
+      </c>
+      <c r="B14" t="s">
+        <v>43</v>
+      </c>
+      <c r="C14" t="s">
+        <v>50</v>
+      </c>
+      <c r="D14" t="s">
         <v>51</v>
       </c>
-      <c r="B14" t="s">
-        <v>50</v>
-      </c>
-      <c r="C14" t="s">
-        <v>57</v>
-      </c>
-      <c r="D14" t="s">
-        <v>58</v>
-      </c>
       <c r="E14" s="3" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
     </row>
     <row r="15" spans="1:7">
       <c r="A15" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="B15" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="C15" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="D15" s="7" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
     </row>
     <row r="16" spans="1:7">
       <c r="A16" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="B16" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="C16" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="D16" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
     </row>
     <row r="17" spans="1:7">
       <c r="A17" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="B17" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="C17" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="D17" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="F17">
         <v>1</v>
       </c>
       <c r="G17" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
     </row>
     <row r="18" spans="1:7">
@@ -1238,19 +1197,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E8" r:id="rId1"/>
-    <hyperlink ref="E9" r:id="rId2"/>
-    <hyperlink ref="E10" r:id="rId3"/>
-    <hyperlink ref="E11" r:id="rId4"/>
-    <hyperlink ref="E12" r:id="rId5"/>
-    <hyperlink ref="E13" r:id="rId6" display="https://www.digikey.com/en/products/detail/adafruit-industries-llc/161/7244927?utm_adgroup=Optical%20Sensors%20-%20Photo%20Detectors%20-%20CdS%20Cells&amp;utm_source=google&amp;utm_medium=cpc&amp;utm_campaign=Shopping_Product_Sensors%2C%20Transducers&amp;utm_term=&amp;utm_content=Optical%20Sensors%20-%20Photo%20Detectors%20-%20CdS%20Cells&amp;gclid=Cj0KCQiA09eQBhCxARIsAAYRiykKKTy26t9RMu3thm4BXJjP05883nAXP3698XRbwioa7IpavDa5CJsaAmxBEALw_wcB"/>
-    <hyperlink ref="E17" r:id="rId7"/>
-    <hyperlink ref="E14" r:id="rId8"/>
-    <hyperlink ref="E15" r:id="rId9"/>
-    <hyperlink ref="E16" r:id="rId10"/>
+    <hyperlink ref="E13" r:id="rId1" display="https://www.digikey.com/en/products/detail/adafruit-industries-llc/161/7244927?utm_adgroup=Optical%20Sensors%20-%20Photo%20Detectors%20-%20CdS%20Cells&amp;utm_source=google&amp;utm_medium=cpc&amp;utm_campaign=Shopping_Product_Sensors%2C%20Transducers&amp;utm_term=&amp;utm_content=Optical%20Sensors%20-%20Photo%20Detectors%20-%20CdS%20Cells&amp;gclid=Cj0KCQiA09eQBhCxARIsAAYRiykKKTy26t9RMu3thm4BXJjP05883nAXP3698XRbwioa7IpavDa5CJsaAmxBEALw_wcB"/>
+    <hyperlink ref="E17" r:id="rId2"/>
+    <hyperlink ref="E14" r:id="rId3"/>
+    <hyperlink ref="E15" r:id="rId4"/>
+    <hyperlink ref="E16" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId11"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId6"/>
 </worksheet>
 </file>
 
@@ -1258,8 +1212,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I112"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K20" sqref="K20"/>
+    <sheetView topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="L47" sqref="L47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1291,16 +1245,16 @@
         <v>5</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>154</v>
+        <v>147</v>
       </c>
     </row>
     <row r="2" spans="1:9">
@@ -1326,7 +1280,7 @@
         <v>1</v>
       </c>
       <c r="H2" s="16" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="I2">
         <v>1</v>
@@ -1355,7 +1309,7 @@
         <v>2</v>
       </c>
       <c r="H3" s="16" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="I3">
         <v>1</v>
@@ -1384,7 +1338,7 @@
         <v>2</v>
       </c>
       <c r="H4" s="16" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="I4">
         <v>1</v>
@@ -1413,7 +1367,7 @@
         <v>2</v>
       </c>
       <c r="H5" s="16" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="I5">
         <v>1</v>
@@ -1442,7 +1396,7 @@
         <v>2</v>
       </c>
       <c r="H6" s="16" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="I6">
         <v>1</v>
@@ -1471,7 +1425,7 @@
         <v>1</v>
       </c>
       <c r="H7" s="18" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="I7">
         <v>1</v>
@@ -1482,16 +1436,16 @@
         <v>2</v>
       </c>
       <c r="B8" s="13" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="C8" s="13" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="D8" s="13" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="E8" s="14" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="F8" s="13">
         <v>1</v>
@@ -1501,7 +1455,7 @@
         <v>2</v>
       </c>
       <c r="H8" s="18" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="I8">
         <v>2</v>
@@ -1512,16 +1466,16 @@
         <v>2</v>
       </c>
       <c r="B9" s="13" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="C9" s="13" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="D9" s="13" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="E9" s="14" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="F9" s="13">
         <v>1</v>
@@ -1531,7 +1485,7 @@
         <v>2</v>
       </c>
       <c r="H9" s="18" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="I9">
         <v>2</v>
@@ -1542,17 +1496,17 @@
         <v>2</v>
       </c>
       <c r="B10" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="C10" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="D10" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="E10" s="14" t="s">
         <v>67</v>
       </c>
-      <c r="C10" s="13" t="s">
-        <v>72</v>
-      </c>
-      <c r="D10" s="13" t="s">
-        <v>73</v>
-      </c>
-      <c r="E10" s="14" t="s">
-        <v>74</v>
-      </c>
       <c r="F10" s="13">
         <v>1</v>
       </c>
@@ -1560,7 +1514,7 @@
         <v>1</v>
       </c>
       <c r="H10" s="18" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="I10">
         <v>2</v>
@@ -1571,16 +1525,16 @@
         <v>2</v>
       </c>
       <c r="B11" s="13" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="C11" s="13" t="s">
         <v>26</v>
       </c>
       <c r="D11" s="13" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="E11" s="14" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="F11" s="13">
         <v>1</v>
@@ -1589,7 +1543,7 @@
         <v>1</v>
       </c>
       <c r="H11" s="18" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="I11">
         <v>2</v>
@@ -1600,16 +1554,16 @@
         <v>2</v>
       </c>
       <c r="B12" s="13" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="C12" s="13" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="D12" s="13" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="E12" s="14" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="F12" s="13">
         <v>4</v>
@@ -1619,7 +1573,7 @@
         <v>5</v>
       </c>
       <c r="H12" s="18" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="I12">
         <v>2</v>
@@ -1630,16 +1584,16 @@
         <v>2</v>
       </c>
       <c r="B13" s="13" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="C13" s="13" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="D13" s="13" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="E13" s="14" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="F13" s="13">
         <v>3</v>
@@ -1649,7 +1603,7 @@
         <v>4</v>
       </c>
       <c r="H13" s="18" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="I13">
         <v>2</v>
@@ -1660,16 +1614,16 @@
         <v>2</v>
       </c>
       <c r="B14" s="13" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="C14" s="13" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="D14" s="13" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="E14" s="14" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="F14" s="13">
         <v>1</v>
@@ -1679,7 +1633,7 @@
         <v>2</v>
       </c>
       <c r="H14" s="18" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="I14">
         <v>2</v>
@@ -1690,16 +1644,16 @@
         <v>2</v>
       </c>
       <c r="B15" s="13" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="C15" s="13" t="s">
         <v>3</v>
       </c>
       <c r="D15" s="13" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="E15" s="14" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="F15" s="13">
         <v>1</v>
@@ -1708,7 +1662,7 @@
         <v>1</v>
       </c>
       <c r="H15" s="18" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="I15">
         <v>2</v>
@@ -1719,16 +1673,16 @@
         <v>2</v>
       </c>
       <c r="B16" s="13" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="C16" s="13" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="D16" s="13" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="E16" s="14" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="F16" s="13">
         <v>2</v>
@@ -1737,7 +1691,7 @@
         <v>2</v>
       </c>
       <c r="H16" s="18" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="I16">
         <v>2</v>
@@ -1748,16 +1702,16 @@
         <v>2</v>
       </c>
       <c r="B17" s="13" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="C17" s="13" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="D17" s="13" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="E17" s="14" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="F17" s="13">
         <v>1</v>
@@ -1766,7 +1720,7 @@
         <v>0</v>
       </c>
       <c r="H17" s="18" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="I17">
         <v>2</v>
@@ -1777,16 +1731,16 @@
         <v>2</v>
       </c>
       <c r="B18" s="13" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="C18" s="13" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="D18" s="13" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="E18" s="14" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="F18" s="13">
         <v>1</v>
@@ -1796,7 +1750,7 @@
         <v>2</v>
       </c>
       <c r="H18" s="18" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="I18">
         <v>2</v>
@@ -1807,16 +1761,16 @@
         <v>2</v>
       </c>
       <c r="B19" s="13" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="C19" s="13" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
       <c r="D19" s="13" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
       <c r="E19" s="14" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
       <c r="F19" s="13">
         <v>1</v>
@@ -1825,7 +1779,7 @@
         <v>10</v>
       </c>
       <c r="H19" s="18" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="I19">
         <v>2</v>
@@ -1836,16 +1790,16 @@
         <v>2</v>
       </c>
       <c r="B20" s="13" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="C20" s="13" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="D20" s="13" t="s">
-        <v>112</v>
+        <v>105</v>
       </c>
       <c r="E20" s="14" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="F20" s="13">
         <v>1</v>
@@ -1854,7 +1808,7 @@
         <v>10</v>
       </c>
       <c r="H20" s="18" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="I20">
         <v>2</v>
@@ -1865,16 +1819,16 @@
         <v>2</v>
       </c>
       <c r="B21" s="13" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="C21" s="13" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
       <c r="D21" s="13" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="E21" s="14" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="F21" s="13">
         <v>1</v>
@@ -1884,7 +1838,7 @@
         <v>2</v>
       </c>
       <c r="H21" s="18" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="I21">
         <v>2</v>
@@ -1895,16 +1849,16 @@
         <v>2</v>
       </c>
       <c r="B22" s="13" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="C22" s="13" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
       <c r="D22" s="13" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
       <c r="E22" s="14" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
       <c r="F22" s="13">
         <v>1</v>
@@ -1913,7 +1867,7 @@
         <v>10</v>
       </c>
       <c r="H22" s="18" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="I22">
         <v>2</v>
@@ -1924,16 +1878,16 @@
         <v>2</v>
       </c>
       <c r="B23" s="13" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="C23" s="13" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="D23" s="13" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
       <c r="E23" s="14" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="F23" s="13">
         <v>1</v>
@@ -1943,7 +1897,7 @@
         <v>2</v>
       </c>
       <c r="H23" s="18" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="I23">
         <v>2</v>
@@ -1954,16 +1908,16 @@
         <v>2</v>
       </c>
       <c r="B24" s="13" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="C24" s="13" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="D24" s="19">
         <v>860160672005</v>
       </c>
       <c r="E24" s="14" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
       <c r="F24" s="13">
         <v>2</v>
@@ -1972,7 +1926,7 @@
         <v>2</v>
       </c>
       <c r="H24" s="18" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="I24">
         <v>2</v>
@@ -1983,16 +1937,16 @@
         <v>2</v>
       </c>
       <c r="B25" s="13" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="C25" s="13" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="D25" s="13" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
       <c r="E25" s="14" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="F25" s="13">
         <v>4</v>
@@ -2001,7 +1955,7 @@
         <v>10</v>
       </c>
       <c r="H25" s="18" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="I25">
         <v>3</v>
@@ -2012,16 +1966,16 @@
         <v>2</v>
       </c>
       <c r="B26" s="13" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="C26" s="13" t="s">
         <v>26</v>
       </c>
       <c r="D26" s="13" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="E26" s="14" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="F26" s="13">
         <v>4</v>
@@ -2030,7 +1984,7 @@
         <v>4</v>
       </c>
       <c r="H26" s="18" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="I26">
         <v>3</v>
@@ -2041,16 +1995,16 @@
         <v>2</v>
       </c>
       <c r="B27" s="13" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="C27" s="13" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="D27" s="13" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="E27" s="14" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="F27" s="13">
         <v>1</v>
@@ -2059,7 +2013,7 @@
         <v>1</v>
       </c>
       <c r="H27" s="18" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="I27">
         <v>3</v>
@@ -2070,16 +2024,16 @@
         <v>2</v>
       </c>
       <c r="B28" s="13" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="C28" s="13" t="s">
+        <v>113</v>
+      </c>
+      <c r="D28" s="13" t="s">
         <v>120</v>
       </c>
-      <c r="D28" s="13" t="s">
-        <v>127</v>
-      </c>
       <c r="E28" s="14" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="F28" s="13">
         <v>2</v>
@@ -2088,7 +2042,7 @@
         <v>2</v>
       </c>
       <c r="H28" s="18" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="I28">
         <v>3</v>
@@ -2099,16 +2053,16 @@
         <v>2</v>
       </c>
       <c r="B29" s="13" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="C29" s="13" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="D29" s="13" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="E29" s="14" t="s">
-        <v>130</v>
+        <v>123</v>
       </c>
       <c r="F29" s="13">
         <v>2</v>
@@ -2118,7 +2072,7 @@
         <v>3</v>
       </c>
       <c r="H29" s="18" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="I29">
         <v>3</v>
@@ -2129,16 +2083,16 @@
         <v>2</v>
       </c>
       <c r="B30" s="13" t="s">
-        <v>133</v>
+        <v>126</v>
       </c>
       <c r="C30" s="13" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
       <c r="D30" s="13" t="s">
-        <v>134</v>
+        <v>127</v>
       </c>
       <c r="E30" s="14" t="s">
-        <v>136</v>
+        <v>129</v>
       </c>
       <c r="F30" s="13">
         <v>1</v>
@@ -2147,7 +2101,7 @@
         <v>1</v>
       </c>
       <c r="H30" s="18" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="I30">
         <v>4</v>
@@ -2158,16 +2112,16 @@
         <v>2</v>
       </c>
       <c r="B31" s="13" t="s">
-        <v>133</v>
+        <v>126</v>
       </c>
       <c r="C31" s="13" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="D31" s="13" t="s">
-        <v>138</v>
+        <v>131</v>
       </c>
       <c r="E31" s="14" t="s">
-        <v>139</v>
+        <v>132</v>
       </c>
       <c r="F31" s="13">
         <v>1</v>
@@ -2176,7 +2130,7 @@
         <v>1</v>
       </c>
       <c r="H31" s="18" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="I31">
         <v>4</v>
@@ -2187,16 +2141,16 @@
         <v>2</v>
       </c>
       <c r="B32" s="13" t="s">
-        <v>133</v>
+        <v>126</v>
       </c>
       <c r="C32" s="13" t="s">
-        <v>145</v>
+        <v>138</v>
       </c>
       <c r="D32" s="13" t="s">
-        <v>146</v>
+        <v>139</v>
       </c>
       <c r="E32" s="14" t="s">
-        <v>149</v>
+        <v>142</v>
       </c>
       <c r="F32" s="13">
         <v>1</v>
@@ -2214,16 +2168,16 @@
         <v>2</v>
       </c>
       <c r="B33" s="13" t="s">
-        <v>133</v>
+        <v>126</v>
       </c>
       <c r="C33" s="13" t="s">
-        <v>145</v>
+        <v>138</v>
       </c>
       <c r="D33" s="13" t="s">
-        <v>147</v>
+        <v>140</v>
       </c>
       <c r="E33" s="14" t="s">
-        <v>148</v>
+        <v>141</v>
       </c>
       <c r="F33" s="13">
         <v>1</v>
@@ -2241,16 +2195,16 @@
         <v>2</v>
       </c>
       <c r="B34" s="13" t="s">
-        <v>140</v>
+        <v>133</v>
       </c>
       <c r="C34" s="13" t="s">
-        <v>141</v>
+        <v>134</v>
       </c>
       <c r="D34" s="13" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="E34" s="14" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="F34" s="13">
         <v>1</v>
@@ -2259,7 +2213,7 @@
         <v>1</v>
       </c>
       <c r="H34" s="18" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="I34">
         <v>5</v>
@@ -2270,16 +2224,16 @@
         <v>2</v>
       </c>
       <c r="B35" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C35" t="s">
         <v>25</v>
       </c>
       <c r="D35" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="F35" s="6">
         <v>1</v>
@@ -2288,7 +2242,7 @@
         <v>0</v>
       </c>
       <c r="H35" s="16" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="I35">
         <v>6</v>
@@ -2296,19 +2250,19 @@
     </row>
     <row r="36" spans="1:9">
       <c r="A36" s="13" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B36" s="13" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C36" s="13" t="s">
-        <v>151</v>
+        <v>144</v>
       </c>
       <c r="D36" s="13" t="s">
-        <v>152</v>
+        <v>145</v>
       </c>
       <c r="E36" s="14" t="s">
-        <v>153</v>
+        <v>146</v>
       </c>
       <c r="F36" s="20">
         <v>4</v>
@@ -2323,19 +2277,19 @@
     </row>
     <row r="37" spans="1:9">
       <c r="A37" t="s">
+        <v>34</v>
+      </c>
+      <c r="B37" t="s">
+        <v>33</v>
+      </c>
+      <c r="C37" t="s">
         <v>36</v>
       </c>
-      <c r="B37" t="s">
-        <v>35</v>
-      </c>
-      <c r="C37" t="s">
-        <v>40</v>
-      </c>
       <c r="D37" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="E37" s="3" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="F37" s="6">
         <v>1</v>
@@ -2349,180 +2303,468 @@
       </c>
     </row>
     <row r="38" spans="1:9">
-      <c r="A38" s="13" t="s">
-        <v>144</v>
-      </c>
-      <c r="B38" s="13" t="s">
-        <v>144</v>
-      </c>
-      <c r="C38" s="13" t="s">
-        <v>150</v>
-      </c>
-      <c r="D38" s="17" t="s">
-        <v>161</v>
-      </c>
-      <c r="E38" s="14" t="s">
-        <v>162</v>
-      </c>
-      <c r="F38" s="13">
-        <v>1</v>
-      </c>
-      <c r="G38" s="13">
-        <v>1</v>
-      </c>
-      <c r="H38" s="18"/>
+      <c r="A38" t="s">
+        <v>34</v>
+      </c>
+      <c r="B38" t="s">
+        <v>33</v>
+      </c>
+      <c r="C38" t="s">
+        <v>156</v>
+      </c>
+      <c r="D38" t="s">
+        <v>35</v>
+      </c>
+      <c r="E38" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="F38">
+        <v>4</v>
+      </c>
+      <c r="G38">
+        <v>4</v>
+      </c>
+      <c r="H38" s="16"/>
       <c r="I38">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="39" spans="1:9">
-      <c r="A39" s="13" t="s">
-        <v>144</v>
-      </c>
-      <c r="B39" s="13" t="s">
-        <v>144</v>
+      <c r="A39" t="s">
+        <v>34</v>
+      </c>
+      <c r="B39" t="s">
+        <v>33</v>
       </c>
       <c r="C39" t="s">
         <v>26</v>
       </c>
-      <c r="D39" t="s">
-        <v>96</v>
-      </c>
-      <c r="E39" s="3" t="s">
-        <v>125</v>
+      <c r="D39" s="13" t="s">
+        <v>89</v>
+      </c>
+      <c r="E39" s="14" t="s">
+        <v>118</v>
       </c>
       <c r="F39">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G39">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H39" s="16"/>
       <c r="I39">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="40" spans="1:9">
-      <c r="A40" s="13" t="s">
-        <v>144</v>
-      </c>
-      <c r="B40" s="13" t="s">
-        <v>144</v>
+      <c r="A40" t="s">
+        <v>34</v>
+      </c>
+      <c r="B40" t="s">
+        <v>33</v>
       </c>
       <c r="C40" t="s">
-        <v>155</v>
-      </c>
-      <c r="D40" s="2" t="s">
-        <v>157</v>
+        <v>96</v>
+      </c>
+      <c r="D40" t="s">
+        <v>107</v>
       </c>
       <c r="E40" s="3" t="s">
-        <v>156</v>
+        <v>108</v>
       </c>
       <c r="F40">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G40">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H40" s="16"/>
       <c r="I40">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="41" spans="1:9">
-      <c r="A41" s="13" t="s">
-        <v>144</v>
-      </c>
-      <c r="B41" s="13" t="s">
-        <v>144</v>
+      <c r="A41" t="s">
+        <v>34</v>
+      </c>
+      <c r="B41" t="s">
+        <v>33</v>
       </c>
       <c r="C41" t="s">
+        <v>160</v>
+      </c>
+      <c r="D41" t="s">
         <v>158</v>
       </c>
-      <c r="D41" s="2" t="s">
+      <c r="E41" s="3" t="s">
         <v>159</v>
       </c>
-      <c r="E41" s="3" t="s">
-        <v>160</v>
-      </c>
       <c r="F41">
         <v>1</v>
       </c>
       <c r="G41">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="H41" s="16"/>
       <c r="I41">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9">
+      <c r="A42" t="s">
+        <v>34</v>
+      </c>
+      <c r="B42" t="s">
+        <v>33</v>
+      </c>
+      <c r="C42" t="s">
+        <v>161</v>
+      </c>
+      <c r="D42" t="s">
+        <v>162</v>
+      </c>
+      <c r="E42" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="F42">
+        <v>2</v>
+      </c>
+      <c r="G42">
+        <v>3</v>
+      </c>
+      <c r="H42" s="16"/>
+      <c r="I42">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9">
+      <c r="A43" t="s">
+        <v>34</v>
+      </c>
+      <c r="B43" t="s">
+        <v>33</v>
+      </c>
+      <c r="C43" t="s">
+        <v>100</v>
+      </c>
+      <c r="D43" t="s">
+        <v>164</v>
+      </c>
+      <c r="E43" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="F43">
+        <v>13</v>
+      </c>
+      <c r="G43">
+        <v>20</v>
+      </c>
+      <c r="H43" s="16"/>
+      <c r="I43">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9">
+      <c r="A44" t="s">
+        <v>2</v>
+      </c>
+      <c r="B44" t="s">
+        <v>33</v>
+      </c>
+      <c r="C44" t="s">
+        <v>167</v>
+      </c>
+      <c r="D44" t="s">
+        <v>39</v>
+      </c>
+      <c r="E44" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F44">
+        <v>1</v>
+      </c>
+      <c r="G44">
+        <v>1</v>
+      </c>
+      <c r="H44" s="16"/>
+      <c r="I44">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9">
+      <c r="A45" t="s">
+        <v>2</v>
+      </c>
+      <c r="B45" t="s">
+        <v>33</v>
+      </c>
+      <c r="C45" t="s">
+        <v>168</v>
+      </c>
+      <c r="D45" t="s">
+        <v>169</v>
+      </c>
+      <c r="E45" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="F45">
+        <v>2</v>
+      </c>
+      <c r="G45">
+        <v>10</v>
+      </c>
+      <c r="H45" s="16"/>
+      <c r="I45">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9">
+      <c r="A46" t="s">
+        <v>2</v>
+      </c>
+      <c r="B46" t="s">
+        <v>33</v>
+      </c>
+      <c r="C46" t="s">
+        <v>174</v>
+      </c>
+      <c r="D46" t="s">
+        <v>175</v>
+      </c>
+      <c r="E46" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="F46">
+        <v>1</v>
+      </c>
+      <c r="G46">
+        <v>1</v>
+      </c>
+      <c r="H46" s="16"/>
+      <c r="I46">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9">
+      <c r="A47" s="13" t="s">
+        <v>137</v>
+      </c>
+      <c r="B47" s="13" t="s">
+        <v>137</v>
+      </c>
+      <c r="C47" s="13" t="s">
+        <v>143</v>
+      </c>
+      <c r="D47" s="17" t="s">
+        <v>154</v>
+      </c>
+      <c r="E47" s="14" t="s">
+        <v>155</v>
+      </c>
+      <c r="F47" s="13">
+        <v>1</v>
+      </c>
+      <c r="G47" s="13">
+        <v>1</v>
+      </c>
+      <c r="H47" s="18"/>
+      <c r="I47">
         <v>7</v>
       </c>
     </row>
-    <row r="42" spans="1:9">
-      <c r="H42" s="16"/>
-    </row>
-    <row r="43" spans="1:9">
-      <c r="H43" s="16"/>
-    </row>
-    <row r="44" spans="1:9">
-      <c r="H44" s="16"/>
-    </row>
-    <row r="45" spans="1:9">
-      <c r="H45" s="16"/>
-    </row>
-    <row r="46" spans="1:9">
-      <c r="H46" s="16"/>
-    </row>
-    <row r="47" spans="1:9">
-      <c r="H47" s="16"/>
-    </row>
     <row r="48" spans="1:9">
+      <c r="A48" s="13" t="s">
+        <v>137</v>
+      </c>
+      <c r="B48" s="13" t="s">
+        <v>137</v>
+      </c>
+      <c r="C48" t="s">
+        <v>26</v>
+      </c>
+      <c r="D48" t="s">
+        <v>89</v>
+      </c>
+      <c r="E48" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="F48">
+        <v>4</v>
+      </c>
+      <c r="G48">
+        <v>4</v>
+      </c>
       <c r="H48" s="16"/>
-    </row>
-    <row r="49" spans="8:8">
+      <c r="I48">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9">
+      <c r="A49" s="13" t="s">
+        <v>137</v>
+      </c>
+      <c r="B49" s="13" t="s">
+        <v>137</v>
+      </c>
+      <c r="C49" t="s">
+        <v>148</v>
+      </c>
+      <c r="D49" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="E49" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="F49">
+        <v>4</v>
+      </c>
+      <c r="G49">
+        <v>4</v>
+      </c>
       <c r="H49" s="16"/>
-    </row>
-    <row r="50" spans="8:8">
+      <c r="I49">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9">
+      <c r="A50" s="13" t="s">
+        <v>137</v>
+      </c>
+      <c r="B50" s="13" t="s">
+        <v>137</v>
+      </c>
+      <c r="C50" t="s">
+        <v>151</v>
+      </c>
+      <c r="D50" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="E50" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="F50">
+        <v>1</v>
+      </c>
+      <c r="G50">
+        <v>2</v>
+      </c>
       <c r="H50" s="16"/>
-    </row>
-    <row r="51" spans="8:8">
+      <c r="I50">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9">
+      <c r="A51" t="s">
+        <v>137</v>
+      </c>
+      <c r="B51" t="s">
+        <v>137</v>
+      </c>
+      <c r="C51" t="s">
+        <v>100</v>
+      </c>
+      <c r="D51" t="s">
+        <v>164</v>
+      </c>
+      <c r="E51" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="F51">
+        <v>6</v>
+      </c>
+      <c r="G51">
+        <v>10</v>
+      </c>
       <c r="H51" s="16"/>
-    </row>
-    <row r="52" spans="8:8">
+      <c r="I51">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9">
+      <c r="A52" t="s">
+        <v>137</v>
+      </c>
+      <c r="B52" t="s">
+        <v>137</v>
+      </c>
+      <c r="C52" t="s">
+        <v>156</v>
+      </c>
+      <c r="D52" t="s">
+        <v>35</v>
+      </c>
+      <c r="E52" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="F52">
+        <v>2</v>
+      </c>
+      <c r="G52">
+        <v>2</v>
+      </c>
       <c r="H52" s="16"/>
-    </row>
-    <row r="53" spans="8:8">
+      <c r="I52">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9">
+      <c r="A53" t="s">
+        <v>2</v>
+      </c>
+      <c r="B53" t="s">
+        <v>166</v>
+      </c>
+      <c r="C53" t="s">
+        <v>171</v>
+      </c>
+      <c r="D53" t="s">
+        <v>172</v>
+      </c>
+      <c r="E53" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="F53">
+        <v>2</v>
+      </c>
+      <c r="G53">
+        <v>2</v>
+      </c>
       <c r="H53" s="16"/>
-    </row>
-    <row r="54" spans="8:8">
+      <c r="I53">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9">
       <c r="H54" s="16"/>
     </row>
-    <row r="55" spans="8:8">
+    <row r="55" spans="1:9">
       <c r="H55" s="16"/>
     </row>
-    <row r="56" spans="8:8">
+    <row r="56" spans="1:9">
       <c r="H56" s="16"/>
     </row>
-    <row r="57" spans="8:8">
+    <row r="57" spans="1:9">
       <c r="H57" s="16"/>
     </row>
-    <row r="58" spans="8:8">
+    <row r="58" spans="1:9">
       <c r="H58" s="16"/>
     </row>
-    <row r="59" spans="8:8">
+    <row r="59" spans="1:9">
       <c r="H59" s="16"/>
     </row>
-    <row r="60" spans="8:8">
+    <row r="60" spans="1:9">
       <c r="H60" s="16"/>
     </row>
-    <row r="61" spans="8:8">
+    <row r="61" spans="1:9">
       <c r="H61" s="16"/>
     </row>
-    <row r="62" spans="8:8">
+    <row r="62" spans="1:9">
       <c r="H62" s="16"/>
     </row>
-    <row r="63" spans="8:8">
+    <row r="63" spans="1:9">
       <c r="H63" s="16"/>
     </row>
-    <row r="64" spans="8:8">
+    <row r="64" spans="1:9">
       <c r="H64" s="16"/>
     </row>
     <row r="65" spans="8:8">
@@ -2709,18 +2951,30 @@
     <hyperlink ref="E34" r:id="rId31"/>
     <hyperlink ref="E33" r:id="rId32"/>
     <hyperlink ref="E32" r:id="rId33"/>
-    <hyperlink ref="E38" r:id="rId34"/>
-    <hyperlink ref="E39" r:id="rId35"/>
+    <hyperlink ref="E47" r:id="rId34"/>
+    <hyperlink ref="E48" r:id="rId35"/>
     <hyperlink ref="E35" r:id="rId36"/>
     <hyperlink ref="E37" r:id="rId37"/>
     <hyperlink ref="E36" r:id="rId38"/>
-    <hyperlink ref="E40" r:id="rId39"/>
-    <hyperlink ref="E41" r:id="rId40"/>
+    <hyperlink ref="E49" r:id="rId39"/>
+    <hyperlink ref="E50" r:id="rId40"/>
+    <hyperlink ref="E38" r:id="rId41"/>
+    <hyperlink ref="E39" r:id="rId42"/>
+    <hyperlink ref="E40" r:id="rId43"/>
+    <hyperlink ref="E41" r:id="rId44"/>
+    <hyperlink ref="E42" r:id="rId45"/>
+    <hyperlink ref="E43" r:id="rId46"/>
+    <hyperlink ref="E44" r:id="rId47"/>
+    <hyperlink ref="E45" r:id="rId48"/>
+    <hyperlink ref="E53" r:id="rId49"/>
+    <hyperlink ref="E51" r:id="rId50"/>
+    <hyperlink ref="E52" r:id="rId51"/>
+    <hyperlink ref="E46" r:id="rId52"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId41"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId53"/>
   <tableParts count="1">
-    <tablePart r:id="rId42"/>
+    <tablePart r:id="rId54"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
finished up MCU board
</commit_message>
<xml_diff>
--- a/datasheets/components.xlsx
+++ b/datasheets/components.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tarko\Desktop\ece445\datasheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5BB6F7E-F003-4411-8B0F-B060C2E9A6E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0983D4D-95DD-4884-B8E8-EAA3F5442FB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3888" yWindow="1452" windowWidth="16728" windowHeight="10908" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="367" uniqueCount="199">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="365" uniqueCount="199">
   <si>
     <t>Board</t>
   </si>
@@ -206,15 +206,6 @@
     <t>GP2Y0A710K0F</t>
   </si>
   <si>
-    <t>https://www.mouser.com/ProductDetail/Vishay-Semiconductors/VOM617A-4X001T?qs=9vrc9xEJKyw%2FVHr4BNAQkg%3D%3D&amp;gclid=Cj0KCQiA09eQBhCxARIsAAYRiymXJ3VqYtSU_p0JwRXYLLoTyvkSZgfF6ZGKDW5ozJThd4Qxth4HsLEaAj_QEALw_wcB</t>
-  </si>
-  <si>
-    <t>Phototransistor</t>
-  </si>
-  <si>
-    <t>VOM617A</t>
-  </si>
-  <si>
     <t>Have 2</t>
   </si>
   <si>
@@ -578,12 +569,6 @@
     <t>0.1uF cap</t>
   </si>
   <si>
-    <t>CL03A104KQ3NNNC</t>
-  </si>
-  <si>
-    <t>https://www.digikey.com/en/products/detail/samsung-electro-mechanics/CL03A104KQ3NNNC/3886671</t>
-  </si>
-  <si>
     <t>22pF cap</t>
   </si>
   <si>
@@ -629,10 +614,25 @@
     <t>oscillator</t>
   </si>
   <si>
-    <t>MXO45HS-3C-16M000000</t>
-  </si>
-  <si>
-    <t>https://www.digikey.com/en/products/detail/cts-frequency-controls/MXO45HS-3C-16M000000/1801865</t>
+    <t>06036C104KAT4A</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/kyocera-avx/06036C104KAT4A/11244654</t>
+  </si>
+  <si>
+    <t>AS-16.000-20-EXT</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/raltron-electronics/AS-16-000-20-EXT/10246238</t>
+  </si>
+  <si>
+    <t>diode</t>
+  </si>
+  <si>
+    <t>SBR80520LT1G</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/onsemi/SBR80520LT1G/5969271</t>
   </si>
 </sst>
 </file>
@@ -1065,10 +1065,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G27"/>
+  <dimension ref="A1:G26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1112,10 +1112,10 @@
         <v>14</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="F2" s="5">
         <v>1</v>
@@ -1126,13 +1126,13 @@
         <v>48</v>
       </c>
       <c r="C3" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="D3" t="s">
-        <v>180</v>
+        <v>192</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>181</v>
+        <v>193</v>
       </c>
       <c r="F3" s="5">
         <v>6</v>
@@ -1143,13 +1143,13 @@
         <v>48</v>
       </c>
       <c r="C4" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="D4" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="F4" s="5">
         <v>2</v>
@@ -1160,13 +1160,13 @@
         <v>48</v>
       </c>
       <c r="C5" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="D5" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="F5" s="5">
         <v>1</v>
@@ -1177,13 +1177,13 @@
         <v>48</v>
       </c>
       <c r="C6" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="D6" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="F6" s="5">
         <v>2</v>
@@ -1194,13 +1194,13 @@
         <v>48</v>
       </c>
       <c r="C7" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="F7" s="5">
         <v>1</v>
@@ -1211,13 +1211,13 @@
         <v>48</v>
       </c>
       <c r="C8" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="D8" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="F8" s="6">
         <v>1</v>
@@ -1228,13 +1228,13 @@
         <v>48</v>
       </c>
       <c r="C9" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="D9" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="F9" s="6">
         <v>1</v>
@@ -1244,8 +1244,18 @@
       <c r="B10" t="s">
         <v>48</v>
       </c>
-      <c r="E10" s="3"/>
-      <c r="F10" s="6"/>
+      <c r="C10" t="s">
+        <v>196</v>
+      </c>
+      <c r="D10" t="s">
+        <v>197</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="F10" s="6">
+        <v>1</v>
+      </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
@@ -1318,86 +1328,69 @@
         <v>44</v>
       </c>
       <c r="B16" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="C16" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="D16" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="E16" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="F16">
+        <v>1</v>
+      </c>
+      <c r="G16" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
-        <v>44</v>
-      </c>
-      <c r="B17" t="s">
-        <v>48</v>
-      </c>
-      <c r="C17" t="s">
-        <v>48</v>
-      </c>
-      <c r="D17" t="s">
-        <v>49</v>
-      </c>
-      <c r="E17" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="F17">
-        <v>1</v>
-      </c>
-      <c r="G17" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="17" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E17" s="3"/>
+    </row>
+    <row r="18" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E18" s="3"/>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="19" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E19" s="3"/>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="20" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E20" s="3"/>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="21" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E21" s="3"/>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="22" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E22" s="3"/>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="23" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E23" s="3"/>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="24" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E24" s="3"/>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="25" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E25" s="3"/>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="26" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E26" s="3"/>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="E27" s="3"/>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="E13" r:id="rId1" display="https://www.digikey.com/en/products/detail/adafruit-industries-llc/161/7244927?utm_adgroup=Optical%20Sensors%20-%20Photo%20Detectors%20-%20CdS%20Cells&amp;utm_source=google&amp;utm_medium=cpc&amp;utm_campaign=Shopping_Product_Sensors%2C%20Transducers&amp;utm_term=&amp;utm_content=Optical%20Sensors%20-%20Photo%20Detectors%20-%20CdS%20Cells&amp;gclid=Cj0KCQiA09eQBhCxARIsAAYRiykKKTy26t9RMu3thm4BXJjP05883nAXP3698XRbwioa7IpavDa5CJsaAmxBEALw_wcB" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="E17" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="E16" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
     <hyperlink ref="E14" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
     <hyperlink ref="E15" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
-    <hyperlink ref="E16" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
-    <hyperlink ref="E3" r:id="rId6" xr:uid="{62F9AA46-5ECB-49E1-87CF-2BAAC61F1C50}"/>
-    <hyperlink ref="E4" r:id="rId7" xr:uid="{D5B5F6EB-BBFA-4BF8-BE3A-18698A8E08B9}"/>
-    <hyperlink ref="E5" r:id="rId8" xr:uid="{2DCC3DD4-0BCA-493A-B095-0FF50278B057}"/>
-    <hyperlink ref="E6" r:id="rId9" xr:uid="{1ED562D4-135D-4B1A-BA50-E822381ED92F}"/>
-    <hyperlink ref="E7" r:id="rId10" xr:uid="{528779E1-B185-456F-9841-7821722FD986}"/>
-    <hyperlink ref="E2" r:id="rId11" xr:uid="{126FD83F-912C-4D4F-B222-61749BD59D2A}"/>
-    <hyperlink ref="E8" r:id="rId12" xr:uid="{A19AF675-7C2F-4B5A-9CA5-7108B48B3DD5}"/>
-    <hyperlink ref="E9" r:id="rId13" xr:uid="{A8934522-DBD8-462A-AD9B-33B5FC017C28}"/>
+    <hyperlink ref="E3" r:id="rId5" xr:uid="{62F9AA46-5ECB-49E1-87CF-2BAAC61F1C50}"/>
+    <hyperlink ref="E4" r:id="rId6" xr:uid="{D5B5F6EB-BBFA-4BF8-BE3A-18698A8E08B9}"/>
+    <hyperlink ref="E5" r:id="rId7" xr:uid="{2DCC3DD4-0BCA-493A-B095-0FF50278B057}"/>
+    <hyperlink ref="E6" r:id="rId8" xr:uid="{1ED562D4-135D-4B1A-BA50-E822381ED92F}"/>
+    <hyperlink ref="E7" r:id="rId9" xr:uid="{528779E1-B185-456F-9841-7821722FD986}"/>
+    <hyperlink ref="E2" r:id="rId10" xr:uid="{126FD83F-912C-4D4F-B222-61749BD59D2A}"/>
+    <hyperlink ref="E8" r:id="rId11" xr:uid="{A19AF675-7C2F-4B5A-9CA5-7108B48B3DD5}"/>
+    <hyperlink ref="E9" r:id="rId12" xr:uid="{A8934522-DBD8-462A-AD9B-33B5FC017C28}"/>
+    <hyperlink ref="E10" r:id="rId13" xr:uid="{B8A0773A-B312-48B1-ABC8-450B5C36FA30}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId14"/>
@@ -1441,16 +1434,16 @@
         <v>5</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
@@ -1476,7 +1469,7 @@
         <v>1</v>
       </c>
       <c r="H2" s="16" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="I2">
         <v>1</v>
@@ -1505,7 +1498,7 @@
         <v>2</v>
       </c>
       <c r="H3" s="16" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="I3">
         <v>1</v>
@@ -1534,7 +1527,7 @@
         <v>2</v>
       </c>
       <c r="H4" s="16" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="I4">
         <v>1</v>
@@ -1563,7 +1556,7 @@
         <v>2</v>
       </c>
       <c r="H5" s="16" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="I5">
         <v>1</v>
@@ -1592,7 +1585,7 @@
         <v>2</v>
       </c>
       <c r="H6" s="16" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="I6">
         <v>1</v>
@@ -1621,7 +1614,7 @@
         <v>1</v>
       </c>
       <c r="H7" s="18" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="I7">
         <v>1</v>
@@ -1632,16 +1625,16 @@
         <v>2</v>
       </c>
       <c r="B8" s="13" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C8" s="13" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="D8" s="13" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="E8" s="14" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="F8" s="13">
         <v>1</v>
@@ -1651,7 +1644,7 @@
         <v>2</v>
       </c>
       <c r="H8" s="18" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="I8">
         <v>2</v>
@@ -1662,16 +1655,16 @@
         <v>2</v>
       </c>
       <c r="B9" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="C9" s="13" t="s">
+        <v>96</v>
+      </c>
+      <c r="D9" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="E9" s="14" t="s">
         <v>60</v>
-      </c>
-      <c r="C9" s="13" t="s">
-        <v>99</v>
-      </c>
-      <c r="D9" s="13" t="s">
-        <v>64</v>
-      </c>
-      <c r="E9" s="14" t="s">
-        <v>63</v>
       </c>
       <c r="F9" s="13">
         <v>1</v>
@@ -1681,7 +1674,7 @@
         <v>2</v>
       </c>
       <c r="H9" s="18" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="I9">
         <v>2</v>
@@ -1692,16 +1685,16 @@
         <v>2</v>
       </c>
       <c r="B10" s="13" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C10" s="13" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="D10" s="13" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="E10" s="14" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="F10" s="13">
         <v>1</v>
@@ -1710,7 +1703,7 @@
         <v>1</v>
       </c>
       <c r="H10" s="18" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="I10">
         <v>2</v>
@@ -1721,16 +1714,16 @@
         <v>2</v>
       </c>
       <c r="B11" s="13" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C11" s="13" t="s">
         <v>26</v>
       </c>
       <c r="D11" s="13" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="E11" s="14" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="F11" s="13">
         <v>1</v>
@@ -1739,7 +1732,7 @@
         <v>1</v>
       </c>
       <c r="H11" s="18" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="I11">
         <v>2</v>
@@ -1750,16 +1743,16 @@
         <v>2</v>
       </c>
       <c r="B12" s="13" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C12" s="13" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="D12" s="13" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="E12" s="14" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="F12" s="13">
         <v>4</v>
@@ -1769,7 +1762,7 @@
         <v>5</v>
       </c>
       <c r="H12" s="18" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="I12">
         <v>2</v>
@@ -1780,16 +1773,16 @@
         <v>2</v>
       </c>
       <c r="B13" s="13" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C13" s="13" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="D13" s="13" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="E13" s="14" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="F13" s="13">
         <v>3</v>
@@ -1799,7 +1792,7 @@
         <v>4</v>
       </c>
       <c r="H13" s="18" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="I13">
         <v>2</v>
@@ -1810,16 +1803,16 @@
         <v>2</v>
       </c>
       <c r="B14" s="13" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C14" s="13" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="D14" s="13" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="E14" s="14" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="F14" s="13">
         <v>1</v>
@@ -1829,7 +1822,7 @@
         <v>2</v>
       </c>
       <c r="H14" s="18" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="I14">
         <v>2</v>
@@ -1840,16 +1833,16 @@
         <v>2</v>
       </c>
       <c r="B15" s="13" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C15" s="13" t="s">
         <v>3</v>
       </c>
       <c r="D15" s="13" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="E15" s="14" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="F15" s="13">
         <v>1</v>
@@ -1858,7 +1851,7 @@
         <v>1</v>
       </c>
       <c r="H15" s="18" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="I15">
         <v>2</v>
@@ -1869,16 +1862,16 @@
         <v>2</v>
       </c>
       <c r="B16" s="13" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C16" s="13" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="D16" s="13" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="E16" s="14" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="F16" s="13">
         <v>2</v>
@@ -1887,7 +1880,7 @@
         <v>2</v>
       </c>
       <c r="H16" s="18" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="I16">
         <v>2</v>
@@ -1898,16 +1891,16 @@
         <v>2</v>
       </c>
       <c r="B17" s="13" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C17" s="13" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="D17" s="13" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="E17" s="14" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="F17" s="13">
         <v>1</v>
@@ -1916,7 +1909,7 @@
         <v>0</v>
       </c>
       <c r="H17" s="18" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="I17">
         <v>2</v>
@@ -1927,16 +1920,16 @@
         <v>2</v>
       </c>
       <c r="B18" s="13" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C18" s="13" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="D18" s="13" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="E18" s="14" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="F18" s="13">
         <v>1</v>
@@ -1946,7 +1939,7 @@
         <v>2</v>
       </c>
       <c r="H18" s="18" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="I18">
         <v>2</v>
@@ -1957,16 +1950,16 @@
         <v>2</v>
       </c>
       <c r="B19" s="13" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C19" s="13" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="D19" s="13" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="E19" s="14" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="F19" s="13">
         <v>1</v>
@@ -1975,7 +1968,7 @@
         <v>10</v>
       </c>
       <c r="H19" s="18" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="I19">
         <v>2</v>
@@ -1986,16 +1979,16 @@
         <v>2</v>
       </c>
       <c r="B20" s="13" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C20" s="13" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="D20" s="13" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="E20" s="14" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="F20" s="13">
         <v>1</v>
@@ -2004,7 +1997,7 @@
         <v>10</v>
       </c>
       <c r="H20" s="18" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="I20">
         <v>2</v>
@@ -2015,16 +2008,16 @@
         <v>2</v>
       </c>
       <c r="B21" s="13" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C21" s="13" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="D21" s="13" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="E21" s="14" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="F21" s="13">
         <v>1</v>
@@ -2034,7 +2027,7 @@
         <v>2</v>
       </c>
       <c r="H21" s="18" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="I21">
         <v>2</v>
@@ -2045,16 +2038,16 @@
         <v>2</v>
       </c>
       <c r="B22" s="13" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C22" s="13" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="D22" s="13" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="E22" s="14" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="F22" s="13">
         <v>1</v>
@@ -2063,7 +2056,7 @@
         <v>10</v>
       </c>
       <c r="H22" s="18" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="I22">
         <v>2</v>
@@ -2074,16 +2067,16 @@
         <v>2</v>
       </c>
       <c r="B23" s="13" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C23" s="13" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="D23" s="13" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="E23" s="14" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="F23" s="13">
         <v>1</v>
@@ -2093,7 +2086,7 @@
         <v>2</v>
       </c>
       <c r="H23" s="18" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="I23">
         <v>2</v>
@@ -2104,16 +2097,16 @@
         <v>2</v>
       </c>
       <c r="B24" s="13" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C24" s="13" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="D24" s="19">
         <v>860160672005</v>
       </c>
       <c r="E24" s="14" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="F24" s="13">
         <v>2</v>
@@ -2122,7 +2115,7 @@
         <v>2</v>
       </c>
       <c r="H24" s="18" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="I24">
         <v>2</v>
@@ -2133,16 +2126,16 @@
         <v>2</v>
       </c>
       <c r="B25" s="13" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="C25" s="13" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="D25" s="13" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="E25" s="14" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="F25" s="13">
         <v>4</v>
@@ -2151,7 +2144,7 @@
         <v>10</v>
       </c>
       <c r="H25" s="18" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="I25">
         <v>3</v>
@@ -2162,16 +2155,16 @@
         <v>2</v>
       </c>
       <c r="B26" s="13" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="C26" s="13" t="s">
         <v>26</v>
       </c>
       <c r="D26" s="13" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="E26" s="14" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="F26" s="13">
         <v>4</v>
@@ -2180,7 +2173,7 @@
         <v>4</v>
       </c>
       <c r="H26" s="18" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="I26">
         <v>3</v>
@@ -2191,16 +2184,16 @@
         <v>2</v>
       </c>
       <c r="B27" s="13" t="s">
+        <v>84</v>
+      </c>
+      <c r="C27" s="13" t="s">
         <v>87</v>
       </c>
-      <c r="C27" s="13" t="s">
-        <v>90</v>
-      </c>
       <c r="D27" s="13" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="E27" s="14" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="F27" s="13">
         <v>1</v>
@@ -2209,7 +2202,7 @@
         <v>1</v>
       </c>
       <c r="H27" s="18" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="I27">
         <v>3</v>
@@ -2220,16 +2213,16 @@
         <v>2</v>
       </c>
       <c r="B28" s="13" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="C28" s="13" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="D28" s="13" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="E28" s="14" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="F28" s="13">
         <v>2</v>
@@ -2238,7 +2231,7 @@
         <v>2</v>
       </c>
       <c r="H28" s="18" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="I28">
         <v>3</v>
@@ -2249,16 +2242,16 @@
         <v>2</v>
       </c>
       <c r="B29" s="13" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="C29" s="13" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="D29" s="13" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="E29" s="14" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="F29" s="13">
         <v>2</v>
@@ -2268,7 +2261,7 @@
         <v>3</v>
       </c>
       <c r="H29" s="18" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="I29">
         <v>3</v>
@@ -2279,17 +2272,17 @@
         <v>2</v>
       </c>
       <c r="B30" s="13" t="s">
+        <v>123</v>
+      </c>
+      <c r="C30" s="13" t="s">
+        <v>125</v>
+      </c>
+      <c r="D30" s="13" t="s">
+        <v>124</v>
+      </c>
+      <c r="E30" s="14" t="s">
         <v>126</v>
       </c>
-      <c r="C30" s="13" t="s">
-        <v>128</v>
-      </c>
-      <c r="D30" s="13" t="s">
-        <v>127</v>
-      </c>
-      <c r="E30" s="14" t="s">
-        <v>129</v>
-      </c>
       <c r="F30" s="13">
         <v>1</v>
       </c>
@@ -2297,7 +2290,7 @@
         <v>1</v>
       </c>
       <c r="H30" s="18" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="I30">
         <v>4</v>
@@ -2308,16 +2301,16 @@
         <v>2</v>
       </c>
       <c r="B31" s="13" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="C31" s="13" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="D31" s="13" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="E31" s="14" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="F31" s="13">
         <v>1</v>
@@ -2326,7 +2319,7 @@
         <v>1</v>
       </c>
       <c r="H31" s="18" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="I31">
         <v>4</v>
@@ -2337,16 +2330,16 @@
         <v>2</v>
       </c>
       <c r="B32" s="13" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="C32" s="13" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="D32" s="13" t="s">
+        <v>136</v>
+      </c>
+      <c r="E32" s="14" t="s">
         <v>139</v>
-      </c>
-      <c r="E32" s="14" t="s">
-        <v>142</v>
       </c>
       <c r="F32" s="13">
         <v>1</v>
@@ -2364,16 +2357,16 @@
         <v>2</v>
       </c>
       <c r="B33" s="13" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="C33" s="13" t="s">
+        <v>135</v>
+      </c>
+      <c r="D33" s="13" t="s">
+        <v>137</v>
+      </c>
+      <c r="E33" s="14" t="s">
         <v>138</v>
-      </c>
-      <c r="D33" s="13" t="s">
-        <v>140</v>
-      </c>
-      <c r="E33" s="14" t="s">
-        <v>141</v>
       </c>
       <c r="F33" s="13">
         <v>1</v>
@@ -2391,10 +2384,10 @@
         <v>2</v>
       </c>
       <c r="B34" s="13" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="C34" s="13" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="D34" s="13" t="s">
         <v>42</v>
@@ -2409,7 +2402,7 @@
         <v>1</v>
       </c>
       <c r="H34" s="18" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="I34">
         <v>5</v>
@@ -2438,7 +2431,7 @@
         <v>0</v>
       </c>
       <c r="H35" s="16" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="I35">
         <v>6</v>
@@ -2452,13 +2445,13 @@
         <v>33</v>
       </c>
       <c r="C36" s="13" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="D36" s="13" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="E36" s="14" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="F36" s="20">
         <v>4</v>
@@ -2506,13 +2499,13 @@
         <v>33</v>
       </c>
       <c r="C38" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="D38" t="s">
         <v>35</v>
       </c>
       <c r="E38" s="3" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="F38">
         <v>4</v>
@@ -2536,10 +2529,10 @@
         <v>26</v>
       </c>
       <c r="D39" s="13" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="E39" s="14" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="F39">
         <v>1</v>
@@ -2560,13 +2553,13 @@
         <v>33</v>
       </c>
       <c r="C40" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="D40" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="E40" s="3" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="F40">
         <v>2</v>
@@ -2587,13 +2580,13 @@
         <v>33</v>
       </c>
       <c r="C41" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="D41" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="E41" s="3" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="F41">
         <v>1</v>
@@ -2614,13 +2607,13 @@
         <v>33</v>
       </c>
       <c r="C42" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="D42" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="E42" s="3" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="F42">
         <v>2</v>
@@ -2641,13 +2634,13 @@
         <v>33</v>
       </c>
       <c r="C43" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="D43" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="E43" s="3" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="F43">
         <v>13</v>
@@ -2668,7 +2661,7 @@
         <v>33</v>
       </c>
       <c r="C44" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="D44" t="s">
         <v>39</v>
@@ -2695,13 +2688,13 @@
         <v>33</v>
       </c>
       <c r="C45" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="D45" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="E45" s="3" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="F45">
         <v>2</v>
@@ -2722,13 +2715,13 @@
         <v>33</v>
       </c>
       <c r="C46" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="D46" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="E46" s="3" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="F46">
         <v>1</v>
@@ -2743,19 +2736,19 @@
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A47" s="13" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="B47" s="13" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="C47" s="13" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="D47" s="17" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="E47" s="14" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="F47" s="13">
         <v>1</v>
@@ -2770,19 +2763,19 @@
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A48" s="13" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="B48" s="13" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="C48" t="s">
         <v>26</v>
       </c>
       <c r="D48" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="E48" s="3" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="F48">
         <v>4</v>
@@ -2797,19 +2790,19 @@
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A49" s="13" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="B49" s="13" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="C49" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="E49" s="3" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="F49">
         <v>4</v>
@@ -2824,19 +2817,19 @@
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A50" s="13" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="B50" s="13" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="C50" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="E50" s="3" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="F50">
         <v>1</v>
@@ -2851,19 +2844,19 @@
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="B51" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="C51" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="D51" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="E51" s="3" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="F51">
         <v>6</v>
@@ -2878,19 +2871,19 @@
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="B52" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="C52" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="D52" t="s">
         <v>35</v>
       </c>
       <c r="E52" s="3" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="F52">
         <v>2</v>
@@ -2908,16 +2901,16 @@
         <v>2</v>
       </c>
       <c r="B53" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="C53" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="D53" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="E53" s="3" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="F53">
         <v>2</v>

</xml_diff>

<commit_message>
finishing up MCU and adding gerbers
</commit_message>
<xml_diff>
--- a/datasheets/components.xlsx
+++ b/datasheets/components.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tarko\Desktop\ece445\datasheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0983D4D-95DD-4884-B8E8-EAA3F5442FB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6EF8F91-D7DB-4691-B3AD-BE5D69B11DF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3888" yWindow="1452" windowWidth="16728" windowHeight="10908" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -749,6 +749,16 @@
   </cellStyles>
   <dxfs count="3">
     <dxf>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
       <font>
         <color rgb="FF006100"/>
       </font>
@@ -757,16 +767,6 @@
           <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -782,7 +782,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table3" displayName="Table3" ref="A1:I112" totalsRowShown="0" headerRowBorderDxfId="2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table3" displayName="Table3" ref="A1:I112" totalsRowShown="0" headerRowBorderDxfId="1">
   <autoFilter ref="A1:I112" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I112">
     <sortCondition ref="I1:I112"/>
@@ -795,7 +795,7 @@
     <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Link"/>
     <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="PCB Quantity"/>
     <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Cart Quantity"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Purchased" dataDxfId="1"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Purchased" dataDxfId="0"/>
     <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Num"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1067,8 +1067,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1135,7 +1135,7 @@
         <v>193</v>
       </c>
       <c r="F3" s="5">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
@@ -3102,7 +3102,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="H1:H1048576">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>